<commit_message>
pages of a song of ice and fire.
</commit_message>
<xml_diff>
--- a/bitmex.xlsx
+++ b/bitmex.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Bitmex</t>
+    <t>BitmexSwap</t>
   </si>
   <si>
     <t>盈利</t>
@@ -50,10 +50,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0%"/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
@@ -1086,12 +1086,12 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.25"/>
+    <col min="1" max="1" width="12.125" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
     <col min="3" max="5" width="9" style="3"/>
     <col min="6" max="6" width="9" style="4"/>
@@ -1137,7 +1137,7 @@
         <v>1.41</v>
       </c>
       <c r="F2" s="8">
-        <f>B2/(E2-B2)</f>
+        <f t="shared" ref="F2:F7" si="0">B2/(E2-B2)</f>
         <v>0.0217391304347826</v>
       </c>
       <c r="H2"/>
@@ -1160,7 +1160,7 @@
         <v>1.13</v>
       </c>
       <c r="F3" s="10">
-        <f>B3/(E3-B3)</f>
+        <f t="shared" si="0"/>
         <v>-0.198581560283688</v>
       </c>
       <c r="H3" t="s">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="I3" s="3">
         <f>SUM(B2:B100)</f>
-        <v>1.55</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1188,7 +1188,7 @@
         <v>1.51</v>
       </c>
       <c r="F4" s="8">
-        <f>B4/(E4-B4)</f>
+        <f t="shared" si="0"/>
         <v>0.336283185840708</v>
       </c>
       <c r="H4" t="s">
@@ -1216,15 +1216,15 @@
         <v>4.33</v>
       </c>
       <c r="F5" s="8">
-        <f>B5/(E5-B5)</f>
+        <f t="shared" si="0"/>
         <v>0.361635220125786</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="11">
-        <f>AVERAGE(F2:F6)</f>
-        <v>0.119512645648447</v>
+        <f>AVERAGE(F2:F100)</f>
+        <v>0.0178454090303426</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B6" s="7">
         <f>E6-E5-D6</f>
-        <v>0.27</v>
+        <v>0.17</v>
       </c>
       <c r="C6" s="3">
         <v>2.25</v>
@@ -1242,18 +1242,34 @@
         <v>-0.8</v>
       </c>
       <c r="E6" s="3">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="F6" s="8">
-        <f>B6/(E6-B6)</f>
-        <v>0.0764872521246458</v>
+        <f t="shared" si="0"/>
+        <v>0.0481586402266289</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:6">
       <c r="A7" s="6">
         <v>43626</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="9">
+        <f>E7-E6-D7</f>
+        <v>-1.71</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.462162162162162</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6">

</xml_diff>